<commit_message>
New java files 25/01/2017
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frameworks\WebdriverTests\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12435" windowWidth="28800" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="testDataSheet" r:id="rId1" sheetId="1"/>
-    <sheet name="userData" r:id="rId2" sheetId="2"/>
+    <sheet name="testDataSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="userData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Locator</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Tooltip of T-shirts link on mouse hover on Women page.</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>MyWishList1</t>
   </si>
   <si>
@@ -72,35 +66,22 @@
     <t>Password1</t>
   </si>
   <si>
-    <t>neeraj@gmail.com</t>
-  </si>
-  <si>
     <t>neeraj2016_1@gmail.com</t>
   </si>
   <si>
-    <t>neeraj2016_2@gmail.com</t>
-  </si>
-  <si>
-    <t>neeraj2016_4@gmail.com</t>
-  </si>
-  <si>
-    <t>neeraj2016_5@gmail.com</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>neeraj2016@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,20 +125,20 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -174,10 +155,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -212,7 +193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,7 +228,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,21 +322,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -372,7 +353,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -424,14 +405,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -440,8 +421,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -470,114 +451,78 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="1" max="1" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A6"/>
-    <hyperlink r:id="rId5" ref="A5"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId6"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>